<commit_message>
updated after round 4 of translation testing
</commit_message>
<xml_diff>
--- a/Talon_modulefiles_stats.xlsx
+++ b/Talon_modulefiles_stats.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="157">
   <si>
     <t xml:space="preserve">Modulefile</t>
   </si>
@@ -42,6 +42,15 @@
     <t xml:space="preserve">Round 1</t>
   </si>
   <si>
+    <t xml:space="preserve">Round2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Round3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Round4</t>
+  </si>
+  <si>
     <t xml:space="preserve">amber</t>
   </si>
   <si>
@@ -318,13 +327,7 @@
     <t xml:space="preserve">warp</t>
   </si>
   <si>
-    <t xml:space="preserve">Round2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Round3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Round4</t>
+    <t xml:space="preserve">Round5</t>
   </si>
   <si>
     <t xml:space="preserve">anaconda</t>
@@ -354,7 +357,7 @@
     <t xml:space="preserve">cmsh</t>
   </si>
   <si>
-    <t xml:space="preserve">Needs to be throughly checked before discussing with DaMiri, might have to be translated manually instead of through the scripts </t>
+    <t xml:space="preserve">Needs to be discussed with DaMiri, might have to be translated manually instead of through the automated scripts</t>
   </si>
   <si>
     <t xml:space="preserve">cuda</t>
@@ -699,15 +702,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -792,10 +795,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K86"/>
+  <dimension ref="A1:M86"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
+      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -804,9 +807,9 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.5"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7704081632653"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="10" min="5" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="114.336734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="12" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="114.336734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -828,597 +831,606 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="4"/>
-      <c r="K4" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="L4" s="4"/>
+      <c r="M4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="6"/>
-      <c r="K5" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="L5" s="6"/>
+      <c r="M5" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="L6" s="4"/>
+      <c r="M6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F7" s="7"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="5" t="s">
-        <v>16</v>
+      <c r="L7" s="8"/>
+      <c r="M7" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="L8" s="4"/>
+      <c r="M8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" s="9"/>
-      <c r="K9" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="L9" s="9"/>
+      <c r="M9" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J10" s="10"/>
-      <c r="K10" s="11"/>
+        <v>23</v>
+      </c>
+      <c r="L10" s="10"/>
+      <c r="M10" s="11"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F65" s="7"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E78" s="12"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F84" s="13"/>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1438,7 +1450,7 @@
   <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L35" activeCellId="0" sqref="L35"/>
+      <selection pane="topLeft" activeCell="L38" activeCellId="0" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1470,347 +1482,350 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>98</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>99</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>100</v>
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="L3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="K4" s="4"/>
       <c r="L4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="K5" s="6"/>
       <c r="L5" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="K6" s="4"/>
       <c r="L6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="K7" s="8"/>
       <c r="L7" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="K8" s="4"/>
       <c r="L8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K9" s="9"/>
       <c r="L9" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="I10" s="14"/>
+      <c r="B10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="I10" s="15"/>
       <c r="K10" s="10"/>
       <c r="L10" s="11"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="I11" s="14"/>
+      <c r="I11" s="15"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="H19" s="15"/>
+        <v>45</v>
+      </c>
+      <c r="H19" s="16"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I24" s="14"/>
+        <v>125</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" s="15"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="H25" s="15"/>
+        <v>126</v>
+      </c>
+      <c r="H25" s="16"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H26" s="15"/>
+        <v>18</v>
+      </c>
+      <c r="H26" s="16"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="H31" s="15"/>
+        <v>132</v>
+      </c>
+      <c r="H31" s="16"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I32" s="14"/>
+        <v>133</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I32" s="15"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I33" s="14"/>
+        <v>10</v>
+      </c>
+      <c r="I33" s="15"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I35" s="0" t="s">
-        <v>136</v>
+        <v>10</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E38" s="12"/>
-      <c r="F38" s="16"/>
+      <c r="F38" s="14"/>
       <c r="G38" s="7"/>
-      <c r="H38" s="0" t="s">
-        <v>136</v>
+      <c r="J38" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="H45" s="15"/>
+        <v>147</v>
+      </c>
+      <c r="H45" s="16"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="I46" s="14"/>
+        <v>148</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="I46" s="15"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1846,15 +1861,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="17" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B2" s="17" t="n">
         <v>1.4</v>
@@ -1863,7 +1878,7 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0"/>
       <c r="B3" s="17" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1878,7 +1893,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="17" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B6" s="17" t="n">
         <v>4.08</v>
@@ -1887,7 +1902,7 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0"/>
       <c r="B7" s="17" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1896,16 +1911,16 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="17" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0"/>
       <c r="B10" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1914,7 +1929,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="17" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B12" s="17" t="n">
         <v>1.4</v>
@@ -1923,7 +1938,7 @@
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0"/>
       <c r="B13" s="17" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1938,10 +1953,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="17" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated stats file about the test rounds performed
</commit_message>
<xml_diff>
--- a/Talon_modulefiles_stats.xlsx
+++ b/Talon_modulefiles_stats.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="162">
   <si>
     <t xml:space="preserve">Modulefile</t>
   </si>
@@ -36,328 +36,343 @@
     <t xml:space="preserve">Remarks</t>
   </si>
   <si>
+    <t xml:space="preserve">Round 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Round 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, Check!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ansys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">armadillo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First attempt at translating and testing Lua modulesfiles as part of migrating from Tcl to Lua, automated via bash shell scripts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bamtools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing Lua versioned modulefiles where Tcl equivalents have an additional method in the modulefile contents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bazel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lua module file load/unload needs to be throughly checked as these contain user group checking logic (achieved by Lua scripts)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcftools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bioperl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bowtie2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify .lua!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bwa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cairo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cd-hit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">circos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cufflinks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ddocent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dlpoly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eigen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">espresso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fastqc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fastxtoolkit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fpart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gamess</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gatk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gaussian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">genenetwork</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gistic2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gnuplot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gromacs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gsl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gulp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hadoop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hisat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">icu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jags</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kallisto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kraken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lammps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mathematica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">matlab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimac2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mpiblast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mplus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">namd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ncurses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nwchem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oncosnp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">openfoam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ovito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paraview</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parsync</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phyml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">picard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">psi4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pytorch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">raxml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sagemath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">samtools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seqprep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sklearn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">soapdenovo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sra-tools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stacks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">star</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stringtie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tdep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tecplot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tensorflow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tophat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trinity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vasp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vcftools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">velvet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">visit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vmd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">warp</t>
+  </si>
+  <si>
     <t xml:space="preserve">Round 0</t>
   </si>
   <si>
-    <t xml:space="preserve">Round 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Round2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Round3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Round4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">amber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ansys</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Legend</t>
-  </si>
-  <si>
-    <t xml:space="preserve">armadillo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bamtools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First attempt at translating and testing Lua modulefiles (Getting Started)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bazel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcftools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
+    <t xml:space="preserve">Round 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Round 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Round 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Round 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">anaconda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bzip2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First attempt at translating and testing Lua modulefiles (Getting Started on Tcl to Lua migration)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster-tools</t>
   </si>
   <si>
     <t xml:space="preserve">Second attempt at translating and testing Lua modulesfiles as part of migrating from Tcl to Lua, automated via bash shell scripts</t>
   </si>
   <si>
-    <t xml:space="preserve">beast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bioperl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Needs to throughly checked before discussing with DaMiri, might have to be translated manually instead of through the scripts </t>
-  </si>
-  <si>
-    <t xml:space="preserve">blast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bowtie2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">verify .lua!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bwa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cairo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cd-hit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">circos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clark</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cufflinks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ddocent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dlpoly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eigen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">espresso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fastqc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fastxtoolkit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fpart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gamess</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gatk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gaussian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">genenetwork</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gistic2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gnuplot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gromacs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gsl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gulp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hadoop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hisat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">icu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jags</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kallisto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">keras</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kraken</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lammps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mathematica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">matlab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">minimac2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mpiblast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mplus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">namd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ncurses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nwchem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oases</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oncosnp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">openfoam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ovito</t>
-  </si>
-  <si>
-    <t xml:space="preserve">paraview</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parsync</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phyml</t>
-  </si>
-  <si>
-    <t xml:space="preserve">picard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plink</t>
-  </si>
-  <si>
-    <t xml:space="preserve">psi4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pytorch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">raxml</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sagemath</t>
-  </si>
-  <si>
-    <t xml:space="preserve">samtools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">seqprep</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sklearn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">soapdenovo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spades</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spark</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spring</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sra-tools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stacks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">star</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stringtie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tdep</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tecplot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tensorflow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tophat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">trinity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vasp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vcftools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">velvet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">visit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vmd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">warp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Round5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">anaconda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">boost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bzip2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cluster-tools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First attempt at translating and testing Lua modulefiles (Getting Started on Tcl to Lua migration)</t>
-  </si>
-  <si>
     <t xml:space="preserve">cmake</t>
   </si>
   <si>
+    <t xml:space="preserve">Third round of testing Lua modulefiles (core utilities)</t>
+  </si>
+  <si>
     <t xml:space="preserve">cmd</t>
   </si>
   <si>
+    <t xml:space="preserve">Round 4 testing of modulefiles that have multiple levels of directories (core utilities)</t>
+  </si>
+  <si>
     <t xml:space="preserve">cmgui</t>
   </si>
   <si>
+    <t xml:space="preserve">Needs to be discussed with DaMiri, might have to be translated manually instead of through the automated scripts</t>
+  </si>
+  <si>
     <t xml:space="preserve">cmsh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Needs to be discussed with DaMiri, might have to be translated manually instead of through the automated scripts</t>
   </si>
   <si>
     <t xml:space="preserve">cuda</t>
@@ -532,7 +547,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -547,8 +562,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF6666FF"/>
-        <bgColor rgb="FF666699"/>
+        <fgColor rgb="FF00CCFF"/>
+        <bgColor rgb="FF33CCCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -559,8 +574,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF99"/>
-        <bgColor rgb="FFFFFF66"/>
+        <fgColor rgb="FF6666FF"/>
+        <bgColor rgb="FF666699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF66"/>
+        <bgColor rgb="FF00FFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -571,8 +592,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00FF66"/>
-        <bgColor rgb="FF00FFFF"/>
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor rgb="FFFFFF66"/>
       </patternFill>
     </fill>
   </fills>
@@ -645,7 +666,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -655,6 +676,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -662,6 +687,26 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -670,15 +715,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -686,19 +735,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -706,11 +751,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -795,21 +844,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M86"/>
+  <dimension ref="A1:L86"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
+      <selection pane="topLeft" activeCell="L21" activeCellId="0" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="12" min="5" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="114.336734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="11" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="111.775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -831,58 +880,57 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="F2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="K3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M3" s="3"/>
+      <c r="L3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="L4" s="4"/>
-      <c r="M4" s="5"/>
+        <v>11</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="L4" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="7"/>
+      <c r="L5" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="L5" s="6"/>
-      <c r="M5" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="8"/>
+      <c r="L6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="4"/>
-      <c r="M6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -891,15 +939,13 @@
       <c r="C7" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="E7" s="9"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>18</v>
@@ -907,57 +953,53 @@
       <c r="C8" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="5"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="11"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="L9" s="9"/>
-      <c r="M9" s="5" t="s">
-        <v>22</v>
-      </c>
+      <c r="K9" s="12"/>
+      <c r="L9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="L10" s="10"/>
-      <c r="M10" s="11"/>
+        <v>21</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>25</v>
+      <c r="D11" s="14" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>18</v>
@@ -965,43 +1007,43 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="E19" s="9"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>18</v>
@@ -1009,17 +1051,17 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>18</v>
@@ -1027,7 +1069,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>18</v>
@@ -1035,30 +1077,31 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F28" s="3"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>18</v>
@@ -1066,17 +1109,17 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>18</v>
@@ -1084,26 +1127,26 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="F36" s="7"/>
+      <c r="E36" s="9"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>18</v>
@@ -1111,7 +1154,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B40" s="0" t="s">
         <v>18</v>
@@ -1119,12 +1162,12 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>18</v>
@@ -1132,30 +1175,31 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B43" s="0" t="s">
-        <v>10</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B47" s="0" t="s">
         <v>18</v>
@@ -1163,25 +1207,26 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="F48" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>18</v>
@@ -1189,7 +1234,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B52" s="0" t="s">
         <v>18</v>
@@ -1197,20 +1242,20 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>25</v>
+        <v>66</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B55" s="0" t="s">
         <v>18</v>
@@ -1218,7 +1263,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B56" s="0" t="s">
         <v>18</v>
@@ -1226,17 +1271,17 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>18</v>
@@ -1244,17 +1289,17 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B62" s="0" t="s">
         <v>18</v>
@@ -1262,7 +1307,7 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B63" s="0" t="s">
         <v>18</v>
@@ -1270,21 +1315,21 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C65" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="F65" s="7"/>
+      <c r="E65" s="9"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B66" s="0" t="s">
         <v>18</v>
@@ -1292,7 +1337,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B67" s="0" t="s">
         <v>18</v>
@@ -1300,17 +1345,17 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B70" s="0" t="s">
         <v>18</v>
@@ -1318,7 +1363,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B71" s="0" t="s">
         <v>18</v>
@@ -1326,7 +1371,7 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B72" s="0" t="s">
         <v>18</v>
@@ -1334,7 +1379,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B73" s="0" t="s">
         <v>18</v>
@@ -1342,17 +1387,17 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B76" s="0" t="s">
         <v>18</v>
@@ -1360,24 +1405,24 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F77" s="3"/>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B78" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E78" s="12"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B79" s="0" t="s">
         <v>18</v>
@@ -1385,7 +1430,7 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B80" s="0" t="s">
         <v>18</v>
@@ -1393,36 +1438,37 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="F81" s="3"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="F84" s="13"/>
+        <v>96</v>
+      </c>
+      <c r="E84" s="15"/>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B86" s="0" t="s">
         <v>18</v>
@@ -1430,7 +1476,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="K3:L3"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1447,19 +1493,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L47"/>
+  <dimension ref="1:47"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L38" activeCellId="0" sqref="L38"/>
+      <selection pane="topLeft" activeCell="C42" activeCellId="0" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.7142857142857"/>
-    <col collapsed="false" hidden="false" max="11" min="3" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="109.75"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="107.316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1476,120 +1522,122 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>101</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>101</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L3" s="3"/>
+        <v>105</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="K4" s="4"/>
-      <c r="L4" s="5"/>
+        <v>106</v>
+      </c>
+      <c r="J4" s="16"/>
+      <c r="K4" s="6" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
+      </c>
+      <c r="J5" s="5"/>
+      <c r="K5" s="6" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="K6" s="4"/>
-      <c r="L6" s="5"/>
+        <v>110</v>
+      </c>
+      <c r="J6" s="17"/>
+      <c r="K6" s="11" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="K7" s="8"/>
-      <c r="L7" s="5" t="s">
-        <v>19</v>
+        <v>112</v>
+      </c>
+      <c r="J7" s="18"/>
+      <c r="K7" s="6" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="K8" s="4"/>
-      <c r="L8" s="5"/>
+        <v>114</v>
+      </c>
+      <c r="J8" s="19"/>
+      <c r="K8" s="6" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="K9" s="9"/>
-      <c r="L9" s="5" t="s">
-        <v>111</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="J9" s="10"/>
+      <c r="K9" s="11"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="I10" s="15"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="11"/>
+        <v>117</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="H10" s="21"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="I11" s="15"/>
+        <v>119</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="H11" s="21"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>18</v>
@@ -1597,7 +1645,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>18</v>
@@ -1608,43 +1656,43 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="H19" s="16"/>
+        <v>43</v>
+      </c>
+      <c r="G19" s="22"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>18</v>
@@ -1652,7 +1700,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>18</v>
@@ -1660,22 +1708,22 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="I24" s="15"/>
+        <v>130</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" s="21"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="H25" s="16"/>
+        <v>131</v>
+      </c>
+      <c r="G25" s="22"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>18</v>
@@ -1683,76 +1731,76 @@
       <c r="C26" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="H26" s="16"/>
+      <c r="G26" s="22"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="H31" s="16"/>
+        <v>137</v>
+      </c>
+      <c r="G31" s="22"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="I32" s="15"/>
+        <v>138</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="H32" s="21"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I33" s="15"/>
+        <v>139</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="H33" s="21"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>137</v>
+        <v>9</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>18</v>
@@ -1760,26 +1808,25 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E38" s="12"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="7"/>
-      <c r="J38" s="2" t="s">
-        <v>137</v>
+        <v>146</v>
+      </c>
+      <c r="E38" s="23"/>
+      <c r="F38" s="9"/>
+      <c r="I38" s="2" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B40" s="0" t="s">
         <v>18</v>
@@ -1787,50 +1834,50 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="H45" s="16"/>
+        <v>152</v>
+      </c>
+      <c r="G45" s="22"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="B46" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D46" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="I46" s="15"/>
+        <v>153</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="H46" s="21"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="J3:K3"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1849,41 +1896,41 @@
   </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J54" activeCellId="0" sqref="J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="17" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="24" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>151</v>
+      <c r="A1" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="17" t="n">
+      <c r="B2" s="24" t="n">
         <v>1.4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0"/>
-      <c r="B3" s="17" t="s">
-        <v>152</v>
+      <c r="B3" s="24" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0"/>
-      <c r="B4" s="17" t="n">
+      <c r="B4" s="24" t="n">
         <v>1.6</v>
       </c>
     </row>
@@ -1892,17 +1939,17 @@
       <c r="B5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="17" t="n">
+      <c r="A6" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="24" t="n">
         <v>4.08</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0"/>
-      <c r="B7" s="17" t="s">
-        <v>153</v>
+      <c r="B7" s="24" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1910,17 +1957,17 @@
       <c r="B8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>154</v>
+      <c r="A9" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0"/>
-      <c r="B10" s="17" t="s">
-        <v>155</v>
+      <c r="B10" s="24" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1928,22 +1975,22 @@
       <c r="B11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="B12" s="17" t="n">
+      <c r="A12" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="24" t="n">
         <v>1.4</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0"/>
-      <c r="B13" s="17" t="s">
-        <v>152</v>
+      <c r="B13" s="24" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0"/>
-      <c r="B14" s="17" t="n">
+      <c r="B14" s="24" t="n">
         <v>1.6</v>
       </c>
     </row>
@@ -1952,11 +1999,11 @@
       <c r="B15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>156</v>
+      <c r="A16" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>